<commit_message>
Add label to confusion matrix colorbar. Update Readme.
</commit_message>
<xml_diff>
--- a/Tables/Regression_Results.xlsx
+++ b/Tables/Regression_Results.xlsx
@@ -475,19 +475,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9040748851485086</v>
+        <v>0.9085909167542987</v>
       </c>
       <c r="D2" t="n">
-        <v>1557358.170258267</v>
+        <v>1404287.212095075</v>
       </c>
       <c r="E2" t="n">
-        <v>1247.941573255041</v>
+        <v>1185.026249538412</v>
       </c>
       <c r="F2" t="n">
-        <v>822.0702927179702</v>
+        <v>796.3903730471892</v>
       </c>
       <c r="G2" t="n">
-        <v>0.437571462660277</v>
+        <v>0.4426531526489699</v>
       </c>
     </row>
     <row r="3">
@@ -500,19 +500,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9599677548029431</v>
+        <v>0.9562354051865986</v>
       </c>
       <c r="D3" t="n">
-        <v>649929.3144234334</v>
+        <v>672340.8512235817</v>
       </c>
       <c r="E3" t="n">
-        <v>806.1819363043514</v>
+        <v>819.9639328797223</v>
       </c>
       <c r="F3" t="n">
-        <v>400.8446421950315</v>
+        <v>391.7746570263255</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1130639482868977</v>
+        <v>0.1104971698303797</v>
       </c>
     </row>
     <row r="4">
@@ -525,19 +525,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9524841413354613</v>
+        <v>0.9554353559330949</v>
       </c>
       <c r="D4" t="n">
-        <v>771426.8658694846</v>
+        <v>684631.7406609196</v>
       </c>
       <c r="E4" t="n">
-        <v>878.3090947209215</v>
+        <v>827.4247643507654</v>
       </c>
       <c r="F4" t="n">
-        <v>435.6455320726733</v>
+        <v>439.7685854653319</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1094570516174347</v>
+        <v>0.1206906508964245</v>
       </c>
     </row>
     <row r="5">
@@ -550,19 +550,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9821133439625952</v>
+        <v>0.9815914795199632</v>
       </c>
       <c r="D5" t="n">
-        <v>290392.4583418807</v>
+        <v>282803.9510495987</v>
       </c>
       <c r="E5" t="n">
-        <v>538.8807459372442</v>
+        <v>531.7931468621974</v>
       </c>
       <c r="F5" t="n">
-        <v>274.6806620365182</v>
+        <v>270.1267558471473</v>
       </c>
       <c r="G5" t="n">
-        <v>0.07076930797172286</v>
+        <v>0.07048792375429497</v>
       </c>
     </row>
     <row r="6">
@@ -575,19 +575,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9821731157673121</v>
+        <v>0.9829774424151519</v>
       </c>
       <c r="D6" t="n">
-        <v>289422.0544119907</v>
+        <v>261511.8660505587</v>
       </c>
       <c r="E6" t="n">
-        <v>537.9796040854994</v>
+        <v>511.3823090903309</v>
       </c>
       <c r="F6" t="n">
-        <v>276.939906137627</v>
+        <v>263.9323708785655</v>
       </c>
       <c r="G6" t="n">
-        <v>0.07359096544436548</v>
+        <v>0.07035621818574513</v>
       </c>
     </row>
     <row r="7">
@@ -600,19 +600,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9759246594843534</v>
+        <v>0.9784192770731999</v>
       </c>
       <c r="D7" t="n">
-        <v>390866.6495926457</v>
+        <v>331537.4376134287</v>
       </c>
       <c r="E7" t="n">
-        <v>625.1932897853636</v>
+        <v>575.7928773555893</v>
       </c>
       <c r="F7" t="n">
-        <v>322.883120725276</v>
+        <v>309.4223596857882</v>
       </c>
       <c r="G7" t="n">
-        <v>0.08876225634328097</v>
+        <v>0.09413805533476534</v>
       </c>
     </row>
     <row r="8">
@@ -625,19 +625,19 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9658102259828125</v>
+        <v>0.9774653775607607</v>
       </c>
       <c r="D8" t="n">
-        <v>555075.946350279</v>
+        <v>346191.8771874636</v>
       </c>
       <c r="E8" t="n">
-        <v>745.0341913967969</v>
+        <v>588.3807246906238</v>
       </c>
       <c r="F8" t="n">
-        <v>513.6313806061189</v>
+        <v>339.5917201842751</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2503237323057665</v>
+        <v>0.1120316488726503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>